<commit_message>
Obsoleting "appraisal of desirability [BCIO:050799]" in favor of "appraisal of desirability [MFOEM:000226]"
</commit_message>
<xml_diff>
--- a/MechanismOfAction/bcio_moa.xlsx
+++ b/MechanismOfAction/bcio_moa.xlsx
@@ -44,12 +44,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ffffff"/>
+        <fgColor rgb="002f4f4f"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="002f4f4f"/>
+        <fgColor rgb="00ffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -1902,62 +1902,62 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>BCIO:050799</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>appraisal of desirability</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr">
+      <c r="C26" s="3" t="inlineStr">
         <is>
           <t>An &lt;emotional-relevance appraisal&gt; of the extent to which something is good or beneficial.</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="D26" s="3" t="inlineStr">
         <is>
           <t>emotional-relevance appraisal</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="2" t="n"/>
-      <c r="H26" s="2" t="n"/>
-      <c r="I26" s="2" t="n"/>
-      <c r="J26" s="2" t="n"/>
-      <c r="K26" s="2" t="n"/>
-      <c r="L26" s="2" t="n"/>
-      <c r="M26" s="2" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N26" s="2" t="n"/>
-      <c r="O26" s="2" t="n"/>
-      <c r="P26" s="2" t="n"/>
-      <c r="Q26" s="2" t="n"/>
-      <c r="R26" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S26" s="2" t="n"/>
-      <c r="T26" s="2" t="n"/>
-      <c r="U26" s="2" t="inlineStr">
+      <c r="E26" s="3" t="n"/>
+      <c r="F26" s="3" t="n"/>
+      <c r="G26" s="3" t="n"/>
+      <c r="H26" s="3" t="n"/>
+      <c r="I26" s="3" t="n"/>
+      <c r="J26" s="3" t="n"/>
+      <c r="K26" s="3" t="n"/>
+      <c r="L26" s="3" t="n"/>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="n"/>
+      <c r="O26" s="3" t="n"/>
+      <c r="P26" s="3" t="n"/>
+      <c r="Q26" s="3" t="n"/>
+      <c r="R26" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S26" s="3" t="n"/>
+      <c r="T26" s="3" t="n"/>
+      <c r="U26" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V26" s="2" t="inlineStr">
-        <is>
-          <t>Published</t>
-        </is>
-      </c>
-      <c r="W26" s="2" t="n"/>
-      <c r="X26" s="2" t="n"/>
+      <c r="V26" s="3" t="inlineStr">
+        <is>
+          <t>Obsolete</t>
+        </is>
+      </c>
+      <c r="W26" s="3" t="n"/>
+      <c r="X26" s="3" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2728,52 +2728,52 @@
       <c r="X40" s="2" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="inlineStr">
+      <c r="A41" s="4" t="inlineStr">
         <is>
           <t>BCIO:050955</t>
         </is>
       </c>
-      <c r="B41" s="3" t="inlineStr">
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>attachment to a caregiver</t>
         </is>
       </c>
-      <c r="C41" s="3" t="inlineStr">
+      <c r="C41" s="4" t="inlineStr">
         <is>
           <t>A &lt;psychological attachment&gt; that is between a caregiver and the care recipient.</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
+      <c r="D41" s="4" t="inlineStr">
         <is>
           <t>psychological attachment</t>
         </is>
       </c>
-      <c r="E41" s="3" t="n"/>
-      <c r="F41" s="3" t="n"/>
-      <c r="G41" s="3" t="n"/>
-      <c r="H41" s="3" t="n"/>
-      <c r="I41" s="3" t="n"/>
-      <c r="J41" s="3" t="n"/>
-      <c r="K41" s="3" t="n"/>
-      <c r="L41" s="3" t="n"/>
-      <c r="M41" s="3" t="n"/>
-      <c r="N41" s="3" t="n"/>
-      <c r="O41" s="3" t="n"/>
-      <c r="P41" s="3" t="n"/>
-      <c r="Q41" s="3" t="n"/>
-      <c r="R41" s="3" t="n">
+      <c r="E41" s="4" t="n"/>
+      <c r="F41" s="4" t="n"/>
+      <c r="G41" s="4" t="n"/>
+      <c r="H41" s="4" t="n"/>
+      <c r="I41" s="4" t="n"/>
+      <c r="J41" s="4" t="n"/>
+      <c r="K41" s="4" t="n"/>
+      <c r="L41" s="4" t="n"/>
+      <c r="M41" s="4" t="n"/>
+      <c r="N41" s="4" t="n"/>
+      <c r="O41" s="4" t="n"/>
+      <c r="P41" s="4" t="n"/>
+      <c r="Q41" s="4" t="n"/>
+      <c r="R41" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S41" s="3" t="n"/>
-      <c r="T41" s="3" t="n"/>
-      <c r="U41" s="3" t="n"/>
-      <c r="V41" s="3" t="inlineStr">
+      <c r="S41" s="4" t="n"/>
+      <c r="T41" s="4" t="n"/>
+      <c r="U41" s="4" t="n"/>
+      <c r="V41" s="4" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="W41" s="3" t="n"/>
-      <c r="X41" s="3" t="n"/>
+      <c r="W41" s="4" t="n"/>
+      <c r="X41" s="4" t="n"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5022,53 +5022,53 @@
       <c r="X77" s="2" t="n"/>
     </row>
     <row r="78">
-      <c r="A78" s="3" t="inlineStr">
+      <c r="A78" s="4" t="inlineStr">
         <is>
           <t>BCIO:050954</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr">
+      <c r="B78" s="4" t="inlineStr">
         <is>
           <t>behavioural substitution capability</t>
         </is>
       </c>
-      <c r="C78" s="3" t="inlineStr">
+      <c r="C78" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">A &lt;behavioural self-regulation capability&gt; concerning substituting a more desired behaviour for a less desired behaviour.
 </t>
         </is>
       </c>
-      <c r="D78" s="3" t="inlineStr">
+      <c r="D78" s="4" t="inlineStr">
         <is>
           <t>behavioural self-regulation capability</t>
         </is>
       </c>
-      <c r="E78" s="3" t="n"/>
-      <c r="F78" s="3" t="n"/>
-      <c r="G78" s="3" t="n"/>
-      <c r="H78" s="3" t="n"/>
-      <c r="I78" s="3" t="n"/>
-      <c r="J78" s="3" t="n"/>
-      <c r="K78" s="3" t="n"/>
-      <c r="L78" s="3" t="n"/>
-      <c r="M78" s="3" t="n"/>
-      <c r="N78" s="3" t="n"/>
-      <c r="O78" s="3" t="n"/>
-      <c r="P78" s="3" t="n"/>
-      <c r="Q78" s="3" t="n"/>
-      <c r="R78" s="3" t="n">
+      <c r="E78" s="4" t="n"/>
+      <c r="F78" s="4" t="n"/>
+      <c r="G78" s="4" t="n"/>
+      <c r="H78" s="4" t="n"/>
+      <c r="I78" s="4" t="n"/>
+      <c r="J78" s="4" t="n"/>
+      <c r="K78" s="4" t="n"/>
+      <c r="L78" s="4" t="n"/>
+      <c r="M78" s="4" t="n"/>
+      <c r="N78" s="4" t="n"/>
+      <c r="O78" s="4" t="n"/>
+      <c r="P78" s="4" t="n"/>
+      <c r="Q78" s="4" t="n"/>
+      <c r="R78" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S78" s="3" t="n"/>
-      <c r="T78" s="3" t="n"/>
-      <c r="U78" s="3" t="n"/>
-      <c r="V78" s="3" t="inlineStr">
+      <c r="S78" s="4" t="n"/>
+      <c r="T78" s="4" t="n"/>
+      <c r="U78" s="4" t="n"/>
+      <c r="V78" s="4" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="W78" s="3" t="n"/>
-      <c r="X78" s="3" t="n"/>
+      <c r="W78" s="4" t="n"/>
+      <c r="X78" s="4" t="n"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -9514,58 +9514,58 @@
       <c r="X150" s="2" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="4" t="inlineStr">
+      <c r="A151" s="3" t="inlineStr">
         <is>
           <t>BCIO:050304</t>
         </is>
       </c>
-      <c r="B151" s="4" t="inlineStr">
+      <c r="B151" s="3" t="inlineStr">
         <is>
           <t>bodily feeling</t>
         </is>
       </c>
-      <c r="C151" s="4" t="inlineStr">
+      <c r="C151" s="3" t="inlineStr">
         <is>
           <t>An affective process involving sensory experience of physiological stimuli.</t>
         </is>
       </c>
-      <c r="D151" s="4" t="inlineStr">
+      <c r="D151" s="3" t="inlineStr">
         <is>
           <t>affective process</t>
         </is>
       </c>
-      <c r="E151" s="4" t="n"/>
-      <c r="F151" s="4" t="n"/>
-      <c r="G151" s="4" t="n"/>
-      <c r="H151" s="4" t="n"/>
-      <c r="I151" s="4" t="n"/>
-      <c r="J151" s="4" t="n"/>
-      <c r="K151" s="4" t="n"/>
-      <c r="L151" s="4" t="n"/>
-      <c r="M151" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N151" s="4" t="n"/>
-      <c r="O151" s="4" t="n"/>
-      <c r="P151" s="4" t="n"/>
-      <c r="Q151" s="4" t="n"/>
-      <c r="R151" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S151" s="4" t="n"/>
-      <c r="T151" s="4" t="n"/>
-      <c r="U151" s="4" t="n"/>
-      <c r="V151" s="4" t="inlineStr">
+      <c r="E151" s="3" t="n"/>
+      <c r="F151" s="3" t="n"/>
+      <c r="G151" s="3" t="n"/>
+      <c r="H151" s="3" t="n"/>
+      <c r="I151" s="3" t="n"/>
+      <c r="J151" s="3" t="n"/>
+      <c r="K151" s="3" t="n"/>
+      <c r="L151" s="3" t="n"/>
+      <c r="M151" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N151" s="3" t="n"/>
+      <c r="O151" s="3" t="n"/>
+      <c r="P151" s="3" t="n"/>
+      <c r="Q151" s="3" t="n"/>
+      <c r="R151" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S151" s="3" t="n"/>
+      <c r="T151" s="3" t="n"/>
+      <c r="U151" s="3" t="n"/>
+      <c r="V151" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W151" s="4" t="n"/>
-      <c r="X151" s="4" t="n"/>
+      <c r="W151" s="3" t="n"/>
+      <c r="X151" s="3" t="n"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -9620,58 +9620,58 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="4" t="inlineStr">
+      <c r="A153" s="3" t="inlineStr">
         <is>
           <t>BCIO:050305</t>
         </is>
       </c>
-      <c r="B153" s="4" t="inlineStr">
+      <c r="B153" s="3" t="inlineStr">
         <is>
           <t>bodily quality</t>
         </is>
       </c>
-      <c r="C153" s="4" t="inlineStr">
+      <c r="C153" s="3" t="inlineStr">
         <is>
           <t>A quality that inheres in some extended organism.</t>
         </is>
       </c>
-      <c r="D153" s="4" t="inlineStr">
+      <c r="D153" s="3" t="inlineStr">
         <is>
           <t>quality</t>
         </is>
       </c>
-      <c r="E153" s="4" t="n"/>
-      <c r="F153" s="4" t="n"/>
-      <c r="G153" s="4" t="n"/>
-      <c r="H153" s="4" t="n"/>
-      <c r="I153" s="4" t="n"/>
-      <c r="J153" s="4" t="n"/>
-      <c r="K153" s="4" t="n"/>
-      <c r="L153" s="4" t="n"/>
-      <c r="M153" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N153" s="4" t="n"/>
-      <c r="O153" s="4" t="n"/>
-      <c r="P153" s="4" t="n"/>
-      <c r="Q153" s="4" t="n"/>
-      <c r="R153" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S153" s="4" t="n"/>
-      <c r="T153" s="4" t="n"/>
-      <c r="U153" s="4" t="n"/>
-      <c r="V153" s="4" t="inlineStr">
+      <c r="E153" s="3" t="n"/>
+      <c r="F153" s="3" t="n"/>
+      <c r="G153" s="3" t="n"/>
+      <c r="H153" s="3" t="n"/>
+      <c r="I153" s="3" t="n"/>
+      <c r="J153" s="3" t="n"/>
+      <c r="K153" s="3" t="n"/>
+      <c r="L153" s="3" t="n"/>
+      <c r="M153" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N153" s="3" t="n"/>
+      <c r="O153" s="3" t="n"/>
+      <c r="P153" s="3" t="n"/>
+      <c r="Q153" s="3" t="n"/>
+      <c r="R153" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S153" s="3" t="n"/>
+      <c r="T153" s="3" t="n"/>
+      <c r="U153" s="3" t="n"/>
+      <c r="V153" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W153" s="4" t="n"/>
-      <c r="X153" s="4" t="n"/>
+      <c r="W153" s="3" t="n"/>
+      <c r="X153" s="3" t="n"/>
     </row>
     <row r="154">
       <c r="A154" s="2" t="inlineStr">
@@ -11805,52 +11805,52 @@
       <c r="X189" s="2" t="n"/>
     </row>
     <row r="190">
-      <c r="A190" s="3" t="inlineStr">
+      <c r="A190" s="4" t="inlineStr">
         <is>
           <t>BCIO:050956</t>
         </is>
       </c>
-      <c r="B190" s="3" t="inlineStr">
+      <c r="B190" s="4" t="inlineStr">
         <is>
           <t>degree of organisational hierarchy</t>
         </is>
       </c>
-      <c r="C190" s="3" t="inlineStr">
+      <c r="C190" s="4" t="inlineStr">
         <is>
           <t>An &lt;organisational attribute&gt; that is the strength and depth of formal authority relations between members of an organisation.</t>
         </is>
       </c>
-      <c r="D190" s="3" t="inlineStr">
+      <c r="D190" s="4" t="inlineStr">
         <is>
           <t>organisational attribute</t>
         </is>
       </c>
-      <c r="E190" s="3" t="n"/>
-      <c r="F190" s="3" t="n"/>
-      <c r="G190" s="3" t="n"/>
-      <c r="H190" s="3" t="n"/>
-      <c r="I190" s="3" t="n"/>
-      <c r="J190" s="3" t="n"/>
-      <c r="K190" s="3" t="n"/>
-      <c r="L190" s="3" t="n"/>
-      <c r="M190" s="3" t="n"/>
-      <c r="N190" s="3" t="n"/>
-      <c r="O190" s="3" t="n"/>
-      <c r="P190" s="3" t="n"/>
-      <c r="Q190" s="3" t="n"/>
-      <c r="R190" s="3" t="n">
+      <c r="E190" s="4" t="n"/>
+      <c r="F190" s="4" t="n"/>
+      <c r="G190" s="4" t="n"/>
+      <c r="H190" s="4" t="n"/>
+      <c r="I190" s="4" t="n"/>
+      <c r="J190" s="4" t="n"/>
+      <c r="K190" s="4" t="n"/>
+      <c r="L190" s="4" t="n"/>
+      <c r="M190" s="4" t="n"/>
+      <c r="N190" s="4" t="n"/>
+      <c r="O190" s="4" t="n"/>
+      <c r="P190" s="4" t="n"/>
+      <c r="Q190" s="4" t="n"/>
+      <c r="R190" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S190" s="3" t="n"/>
-      <c r="T190" s="3" t="n"/>
-      <c r="U190" s="3" t="n"/>
-      <c r="V190" s="3" t="inlineStr">
+      <c r="S190" s="4" t="n"/>
+      <c r="T190" s="4" t="n"/>
+      <c r="U190" s="4" t="n"/>
+      <c r="V190" s="4" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="W190" s="3" t="n"/>
-      <c r="X190" s="3" t="n"/>
+      <c r="W190" s="4" t="n"/>
+      <c r="X190" s="4" t="n"/>
     </row>
     <row r="191">
       <c r="A191" s="2" t="inlineStr">
@@ -15863,62 +15863,62 @@
       <c r="X257" s="2" t="n"/>
     </row>
     <row r="258">
-      <c r="A258" s="4" t="inlineStr">
+      <c r="A258" s="3" t="inlineStr">
         <is>
           <t>BCIO:050657</t>
         </is>
       </c>
-      <c r="B258" s="4" t="inlineStr">
+      <c r="B258" s="3" t="inlineStr">
         <is>
           <t>family behavioural consequence</t>
         </is>
       </c>
-      <c r="C258" s="4" t="inlineStr">
+      <c r="C258" s="3" t="inlineStr">
         <is>
           <t>A &lt;social behavioural consequence&gt; of some family member.</t>
         </is>
       </c>
-      <c r="D258" s="4" t="inlineStr">
+      <c r="D258" s="3" t="inlineStr">
         <is>
           <t>social behavioural consequence</t>
         </is>
       </c>
-      <c r="E258" s="4" t="n"/>
-      <c r="F258" s="4" t="n"/>
-      <c r="G258" s="4" t="n"/>
-      <c r="H258" s="4" t="n"/>
-      <c r="I258" s="4" t="n"/>
-      <c r="J258" s="4" t="n"/>
-      <c r="K258" s="4" t="n"/>
-      <c r="L258" s="4" t="n"/>
-      <c r="M258" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N258" s="4" t="n"/>
-      <c r="O258" s="4" t="n"/>
-      <c r="P258" s="4" t="n"/>
-      <c r="Q258" s="4" t="n"/>
-      <c r="R258" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S258" s="4" t="n"/>
-      <c r="T258" s="4" t="n"/>
-      <c r="U258" s="4" t="inlineStr">
+      <c r="E258" s="3" t="n"/>
+      <c r="F258" s="3" t="n"/>
+      <c r="G258" s="3" t="n"/>
+      <c r="H258" s="3" t="n"/>
+      <c r="I258" s="3" t="n"/>
+      <c r="J258" s="3" t="n"/>
+      <c r="K258" s="3" t="n"/>
+      <c r="L258" s="3" t="n"/>
+      <c r="M258" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N258" s="3" t="n"/>
+      <c r="O258" s="3" t="n"/>
+      <c r="P258" s="3" t="n"/>
+      <c r="Q258" s="3" t="n"/>
+      <c r="R258" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S258" s="3" t="n"/>
+      <c r="T258" s="3" t="n"/>
+      <c r="U258" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V258" s="4" t="inlineStr">
+      <c r="V258" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W258" s="4" t="n"/>
-      <c r="X258" s="4" t="n"/>
+      <c r="W258" s="3" t="n"/>
+      <c r="X258" s="3" t="n"/>
     </row>
     <row r="259">
       <c r="A259" s="2" t="inlineStr">
@@ -22144,62 +22144,62 @@
       <c r="X363" s="2" t="n"/>
     </row>
     <row r="364">
-      <c r="A364" s="4" t="inlineStr">
+      <c r="A364" s="3" t="inlineStr">
         <is>
           <t>BCIO:050696</t>
         </is>
       </c>
-      <c r="B364" s="4" t="inlineStr">
+      <c r="B364" s="3" t="inlineStr">
         <is>
           <t>low motivation to change behaviour</t>
         </is>
       </c>
-      <c r="C364" s="4" t="inlineStr">
+      <c r="C364" s="3" t="inlineStr">
         <is>
           <t>An &lt;attribute&gt; of motivation to change behaviour that is low.</t>
         </is>
       </c>
-      <c r="D364" s="4" t="inlineStr">
+      <c r="D364" s="3" t="inlineStr">
         <is>
           <t>attribute</t>
         </is>
       </c>
-      <c r="E364" s="4" t="n"/>
-      <c r="F364" s="4" t="n"/>
-      <c r="G364" s="4" t="n"/>
-      <c r="H364" s="4" t="n"/>
-      <c r="I364" s="4" t="n"/>
-      <c r="J364" s="4" t="n"/>
-      <c r="K364" s="4" t="n"/>
-      <c r="L364" s="4" t="n"/>
-      <c r="M364" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N364" s="4" t="n"/>
-      <c r="O364" s="4" t="n"/>
-      <c r="P364" s="4" t="n"/>
-      <c r="Q364" s="4" t="n"/>
-      <c r="R364" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S364" s="4" t="n"/>
-      <c r="T364" s="4" t="n"/>
-      <c r="U364" s="4" t="inlineStr">
+      <c r="E364" s="3" t="n"/>
+      <c r="F364" s="3" t="n"/>
+      <c r="G364" s="3" t="n"/>
+      <c r="H364" s="3" t="n"/>
+      <c r="I364" s="3" t="n"/>
+      <c r="J364" s="3" t="n"/>
+      <c r="K364" s="3" t="n"/>
+      <c r="L364" s="3" t="n"/>
+      <c r="M364" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N364" s="3" t="n"/>
+      <c r="O364" s="3" t="n"/>
+      <c r="P364" s="3" t="n"/>
+      <c r="Q364" s="3" t="n"/>
+      <c r="R364" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S364" s="3" t="n"/>
+      <c r="T364" s="3" t="n"/>
+      <c r="U364" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V364" s="4" t="inlineStr">
+      <c r="V364" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W364" s="4" t="n"/>
-      <c r="X364" s="4" t="n"/>
+      <c r="W364" s="3" t="n"/>
+      <c r="X364" s="3" t="n"/>
     </row>
     <row r="365">
       <c r="A365" s="2" t="inlineStr">
@@ -24073,58 +24073,58 @@
       <c r="X395" s="2" t="n"/>
     </row>
     <row r="396">
-      <c r="A396" s="4" t="inlineStr">
+      <c r="A396" s="3" t="inlineStr">
         <is>
           <t>BCIO:050307</t>
         </is>
       </c>
-      <c r="B396" s="4" t="inlineStr">
+      <c r="B396" s="3" t="inlineStr">
         <is>
           <t>mental quality</t>
         </is>
       </c>
-      <c r="C396" s="4" t="inlineStr">
+      <c r="C396" s="3" t="inlineStr">
         <is>
           <t>A bodily quality that inheres in those structures of the extended organism that are essential for mental functioning.</t>
         </is>
       </c>
-      <c r="D396" s="4" t="inlineStr">
+      <c r="D396" s="3" t="inlineStr">
         <is>
           <t>bodily quality</t>
         </is>
       </c>
-      <c r="E396" s="4" t="n"/>
-      <c r="F396" s="4" t="n"/>
-      <c r="G396" s="4" t="n"/>
-      <c r="H396" s="4" t="n"/>
-      <c r="I396" s="4" t="n"/>
-      <c r="J396" s="4" t="n"/>
-      <c r="K396" s="4" t="n"/>
-      <c r="L396" s="4" t="n"/>
-      <c r="M396" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N396" s="4" t="n"/>
-      <c r="O396" s="4" t="n"/>
-      <c r="P396" s="4" t="n"/>
-      <c r="Q396" s="4" t="n"/>
-      <c r="R396" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S396" s="4" t="n"/>
-      <c r="T396" s="4" t="n"/>
-      <c r="U396" s="4" t="n"/>
-      <c r="V396" s="4" t="inlineStr">
+      <c r="E396" s="3" t="n"/>
+      <c r="F396" s="3" t="n"/>
+      <c r="G396" s="3" t="n"/>
+      <c r="H396" s="3" t="n"/>
+      <c r="I396" s="3" t="n"/>
+      <c r="J396" s="3" t="n"/>
+      <c r="K396" s="3" t="n"/>
+      <c r="L396" s="3" t="n"/>
+      <c r="M396" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N396" s="3" t="n"/>
+      <c r="O396" s="3" t="n"/>
+      <c r="P396" s="3" t="n"/>
+      <c r="Q396" s="3" t="n"/>
+      <c r="R396" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S396" s="3" t="n"/>
+      <c r="T396" s="3" t="n"/>
+      <c r="U396" s="3" t="n"/>
+      <c r="V396" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W396" s="4" t="n"/>
-      <c r="X396" s="4" t="n"/>
+      <c r="W396" s="3" t="n"/>
+      <c r="X396" s="3" t="n"/>
     </row>
     <row r="397">
       <c r="A397" s="2" t="inlineStr">
@@ -24632,62 +24632,62 @@
       <c r="X405" s="2" t="n"/>
     </row>
     <row r="406">
-      <c r="A406" s="4" t="inlineStr">
+      <c r="A406" s="3" t="inlineStr">
         <is>
           <t>BCIO:050710</t>
         </is>
       </c>
-      <c r="B406" s="4" t="inlineStr">
+      <c r="B406" s="3" t="inlineStr">
         <is>
           <t>motivation orientation</t>
         </is>
       </c>
-      <c r="C406" s="4" t="inlineStr">
+      <c r="C406" s="3" t="inlineStr">
         <is>
           <t>A &lt;motivational disposition&gt; to be guided by a type of outcome.</t>
         </is>
       </c>
-      <c r="D406" s="4" t="inlineStr">
+      <c r="D406" s="3" t="inlineStr">
         <is>
           <t>motivational disposition</t>
         </is>
       </c>
-      <c r="E406" s="4" t="n"/>
-      <c r="F406" s="4" t="n"/>
-      <c r="G406" s="4" t="n"/>
-      <c r="H406" s="4" t="n"/>
-      <c r="I406" s="4" t="n"/>
-      <c r="J406" s="4" t="n"/>
-      <c r="K406" s="4" t="n"/>
-      <c r="L406" s="4" t="n"/>
-      <c r="M406" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N406" s="4" t="n"/>
-      <c r="O406" s="4" t="n"/>
-      <c r="P406" s="4" t="n"/>
-      <c r="Q406" s="4" t="n"/>
-      <c r="R406" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S406" s="4" t="n"/>
-      <c r="T406" s="4" t="n"/>
-      <c r="U406" s="4" t="inlineStr">
+      <c r="E406" s="3" t="n"/>
+      <c r="F406" s="3" t="n"/>
+      <c r="G406" s="3" t="n"/>
+      <c r="H406" s="3" t="n"/>
+      <c r="I406" s="3" t="n"/>
+      <c r="J406" s="3" t="n"/>
+      <c r="K406" s="3" t="n"/>
+      <c r="L406" s="3" t="n"/>
+      <c r="M406" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N406" s="3" t="n"/>
+      <c r="O406" s="3" t="n"/>
+      <c r="P406" s="3" t="n"/>
+      <c r="Q406" s="3" t="n"/>
+      <c r="R406" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S406" s="3" t="n"/>
+      <c r="T406" s="3" t="n"/>
+      <c r="U406" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V406" s="4" t="inlineStr">
+      <c r="V406" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W406" s="4" t="n"/>
-      <c r="X406" s="4" t="n"/>
+      <c r="W406" s="3" t="n"/>
+      <c r="X406" s="3" t="n"/>
     </row>
     <row r="407">
       <c r="A407" s="2" t="inlineStr">
@@ -27065,52 +27065,52 @@
       <c r="X445" s="2" t="n"/>
     </row>
     <row r="446">
-      <c r="A446" s="3" t="inlineStr">
+      <c r="A446" s="4" t="inlineStr">
         <is>
           <t>BCIO:050957</t>
         </is>
       </c>
-      <c r="B446" s="3" t="inlineStr">
+      <c r="B446" s="4" t="inlineStr">
         <is>
           <t>organisational attribute</t>
         </is>
       </c>
-      <c r="C446" s="3" t="inlineStr">
+      <c r="C446" s="4" t="inlineStr">
         <is>
           <t>A &lt;characteristic&gt; that inheres in an organisation.</t>
         </is>
       </c>
-      <c r="D446" s="3" t="inlineStr">
+      <c r="D446" s="4" t="inlineStr">
         <is>
           <t>characteristic</t>
         </is>
       </c>
-      <c r="E446" s="3" t="n"/>
-      <c r="F446" s="3" t="n"/>
-      <c r="G446" s="3" t="n"/>
-      <c r="H446" s="3" t="n"/>
-      <c r="I446" s="3" t="n"/>
-      <c r="J446" s="3" t="n"/>
-      <c r="K446" s="3" t="n"/>
-      <c r="L446" s="3" t="n"/>
-      <c r="M446" s="3" t="n"/>
-      <c r="N446" s="3" t="n"/>
-      <c r="O446" s="3" t="n"/>
-      <c r="P446" s="3" t="n"/>
-      <c r="Q446" s="3" t="n"/>
-      <c r="R446" s="3" t="n">
+      <c r="E446" s="4" t="n"/>
+      <c r="F446" s="4" t="n"/>
+      <c r="G446" s="4" t="n"/>
+      <c r="H446" s="4" t="n"/>
+      <c r="I446" s="4" t="n"/>
+      <c r="J446" s="4" t="n"/>
+      <c r="K446" s="4" t="n"/>
+      <c r="L446" s="4" t="n"/>
+      <c r="M446" s="4" t="n"/>
+      <c r="N446" s="4" t="n"/>
+      <c r="O446" s="4" t="n"/>
+      <c r="P446" s="4" t="n"/>
+      <c r="Q446" s="4" t="n"/>
+      <c r="R446" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="S446" s="3" t="n"/>
-      <c r="T446" s="3" t="n"/>
-      <c r="U446" s="3" t="n"/>
-      <c r="V446" s="3" t="inlineStr">
+      <c r="S446" s="4" t="n"/>
+      <c r="T446" s="4" t="n"/>
+      <c r="U446" s="4" t="n"/>
+      <c r="V446" s="4" t="inlineStr">
         <is>
           <t>Proposed</t>
         </is>
       </c>
-      <c r="W446" s="3" t="n"/>
-      <c r="X446" s="3" t="n"/>
+      <c r="W446" s="4" t="n"/>
+      <c r="X446" s="4" t="n"/>
     </row>
     <row r="447">
       <c r="A447" s="2" t="inlineStr">
@@ -27684,170 +27684,170 @@
       </c>
     </row>
     <row r="456">
-      <c r="A456" s="4" t="inlineStr">
+      <c r="A456" s="3" t="inlineStr">
         <is>
           <t>BCIO:050301</t>
         </is>
       </c>
-      <c r="B456" s="4" t="inlineStr">
+      <c r="B456" s="3" t="inlineStr">
         <is>
           <t>personal disposition</t>
         </is>
       </c>
-      <c r="C456" s="4" t="inlineStr">
+      <c r="C456" s="3" t="inlineStr">
         <is>
           <t>A disposition that inheres in a person.</t>
         </is>
       </c>
-      <c r="D456" s="4" t="inlineStr">
+      <c r="D456" s="3" t="inlineStr">
         <is>
           <t>disposition</t>
         </is>
       </c>
-      <c r="E456" s="4" t="n"/>
-      <c r="F456" s="4" t="inlineStr">
+      <c r="E456" s="3" t="n"/>
+      <c r="F456" s="3" t="inlineStr">
         <is>
           <t>A characteristic of a person such as intelligence and personality that causes them to think feel or act in a particular way in a particular situation.</t>
         </is>
       </c>
-      <c r="G456" s="4" t="n"/>
-      <c r="H456" s="4" t="n"/>
-      <c r="I456" s="4" t="n"/>
-      <c r="J456" s="4" t="n"/>
-      <c r="K456" s="4" t="n"/>
-      <c r="L456" s="4" t="n"/>
-      <c r="M456" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N456" s="4" t="n"/>
-      <c r="O456" s="4" t="n"/>
-      <c r="P456" s="4" t="n"/>
-      <c r="Q456" s="4" t="n"/>
-      <c r="R456" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S456" s="4" t="n"/>
-      <c r="T456" s="4" t="n"/>
-      <c r="U456" s="4" t="n"/>
-      <c r="V456" s="4" t="inlineStr">
+      <c r="G456" s="3" t="n"/>
+      <c r="H456" s="3" t="n"/>
+      <c r="I456" s="3" t="n"/>
+      <c r="J456" s="3" t="n"/>
+      <c r="K456" s="3" t="n"/>
+      <c r="L456" s="3" t="n"/>
+      <c r="M456" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N456" s="3" t="n"/>
+      <c r="O456" s="3" t="n"/>
+      <c r="P456" s="3" t="n"/>
+      <c r="Q456" s="3" t="n"/>
+      <c r="R456" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S456" s="3" t="n"/>
+      <c r="T456" s="3" t="n"/>
+      <c r="U456" s="3" t="n"/>
+      <c r="V456" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W456" s="4" t="n"/>
-      <c r="X456" s="4" t="n"/>
+      <c r="W456" s="3" t="n"/>
+      <c r="X456" s="3" t="n"/>
     </row>
     <row r="457">
-      <c r="A457" s="4" t="inlineStr">
+      <c r="A457" s="3" t="inlineStr">
         <is>
           <t>BCIO:050302</t>
         </is>
       </c>
-      <c r="B457" s="4" t="inlineStr">
+      <c r="B457" s="3" t="inlineStr">
         <is>
           <t>personal life attribute</t>
         </is>
       </c>
-      <c r="C457" s="4" t="inlineStr">
+      <c r="C457" s="3" t="inlineStr">
         <is>
           <t>A process attribute that is an attribute of a life process.</t>
         </is>
       </c>
-      <c r="D457" s="4" t="inlineStr">
+      <c r="D457" s="3" t="inlineStr">
         <is>
           <t>process attribute</t>
         </is>
       </c>
-      <c r="E457" s="4" t="n"/>
-      <c r="F457" s="4" t="n"/>
-      <c r="G457" s="4" t="n"/>
-      <c r="H457" s="4" t="n"/>
-      <c r="I457" s="4" t="n"/>
-      <c r="J457" s="4" t="n"/>
-      <c r="K457" s="4" t="n"/>
-      <c r="L457" s="4" t="n"/>
-      <c r="M457" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N457" s="4" t="n"/>
-      <c r="O457" s="4" t="n"/>
-      <c r="P457" s="4" t="n"/>
-      <c r="Q457" s="4" t="n"/>
-      <c r="R457" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S457" s="4" t="n"/>
-      <c r="T457" s="4" t="n"/>
-      <c r="U457" s="4" t="n"/>
-      <c r="V457" s="4" t="inlineStr">
+      <c r="E457" s="3" t="n"/>
+      <c r="F457" s="3" t="n"/>
+      <c r="G457" s="3" t="n"/>
+      <c r="H457" s="3" t="n"/>
+      <c r="I457" s="3" t="n"/>
+      <c r="J457" s="3" t="n"/>
+      <c r="K457" s="3" t="n"/>
+      <c r="L457" s="3" t="n"/>
+      <c r="M457" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N457" s="3" t="n"/>
+      <c r="O457" s="3" t="n"/>
+      <c r="P457" s="3" t="n"/>
+      <c r="Q457" s="3" t="n"/>
+      <c r="R457" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S457" s="3" t="n"/>
+      <c r="T457" s="3" t="n"/>
+      <c r="U457" s="3" t="n"/>
+      <c r="V457" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W457" s="4" t="n"/>
-      <c r="X457" s="4" t="n"/>
+      <c r="W457" s="3" t="n"/>
+      <c r="X457" s="3" t="n"/>
     </row>
     <row r="458">
-      <c r="A458" s="4" t="inlineStr">
+      <c r="A458" s="3" t="inlineStr">
         <is>
           <t>BCIO:050303</t>
         </is>
       </c>
-      <c r="B458" s="4" t="inlineStr">
+      <c r="B458" s="3" t="inlineStr">
         <is>
           <t>personal quality</t>
         </is>
       </c>
-      <c r="C458" s="4" t="inlineStr">
+      <c r="C458" s="3" t="inlineStr">
         <is>
           <t>A quality that inheres in a person.</t>
         </is>
       </c>
-      <c r="D458" s="4" t="inlineStr">
+      <c r="D458" s="3" t="inlineStr">
         <is>
           <t>quality</t>
         </is>
       </c>
-      <c r="E458" s="4" t="n"/>
-      <c r="F458" s="4" t="n"/>
-      <c r="G458" s="4" t="n"/>
-      <c r="H458" s="4" t="n"/>
-      <c r="I458" s="4" t="n"/>
-      <c r="J458" s="4" t="n"/>
-      <c r="K458" s="4" t="n"/>
-      <c r="L458" s="4" t="n"/>
-      <c r="M458" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N458" s="4" t="n"/>
-      <c r="O458" s="4" t="n"/>
-      <c r="P458" s="4" t="n"/>
-      <c r="Q458" s="4" t="n"/>
-      <c r="R458" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S458" s="4" t="n"/>
-      <c r="T458" s="4" t="n"/>
-      <c r="U458" s="4" t="n"/>
-      <c r="V458" s="4" t="inlineStr">
+      <c r="E458" s="3" t="n"/>
+      <c r="F458" s="3" t="n"/>
+      <c r="G458" s="3" t="n"/>
+      <c r="H458" s="3" t="n"/>
+      <c r="I458" s="3" t="n"/>
+      <c r="J458" s="3" t="n"/>
+      <c r="K458" s="3" t="n"/>
+      <c r="L458" s="3" t="n"/>
+      <c r="M458" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N458" s="3" t="n"/>
+      <c r="O458" s="3" t="n"/>
+      <c r="P458" s="3" t="n"/>
+      <c r="Q458" s="3" t="n"/>
+      <c r="R458" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S458" s="3" t="n"/>
+      <c r="T458" s="3" t="n"/>
+      <c r="U458" s="3" t="n"/>
+      <c r="V458" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W458" s="4" t="n"/>
-      <c r="X458" s="4" t="n"/>
+      <c r="W458" s="3" t="n"/>
+      <c r="X458" s="3" t="n"/>
     </row>
     <row r="459">
       <c r="A459" s="2" t="inlineStr">
@@ -33368,62 +33368,62 @@
       <c r="X550" s="2" t="n"/>
     </row>
     <row r="551">
-      <c r="A551" s="4" t="inlineStr">
+      <c r="A551" s="3" t="inlineStr">
         <is>
           <t>BCIO:050770</t>
         </is>
       </c>
-      <c r="B551" s="4" t="inlineStr">
+      <c r="B551" s="3" t="inlineStr">
         <is>
           <t>social behavioural consequence</t>
         </is>
       </c>
-      <c r="C551" s="4" t="inlineStr">
+      <c r="C551" s="3" t="inlineStr">
         <is>
           <t>A &lt;behavioural consequence&gt; of a member of the person’s social environmental system.</t>
         </is>
       </c>
-      <c r="D551" s="4" t="inlineStr">
+      <c r="D551" s="3" t="inlineStr">
         <is>
           <t>behavioural consequence</t>
         </is>
       </c>
-      <c r="E551" s="4" t="n"/>
-      <c r="F551" s="4" t="n"/>
-      <c r="G551" s="4" t="n"/>
-      <c r="H551" s="4" t="n"/>
-      <c r="I551" s="4" t="n"/>
-      <c r="J551" s="4" t="n"/>
-      <c r="K551" s="4" t="n"/>
-      <c r="L551" s="4" t="n"/>
-      <c r="M551" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N551" s="4" t="n"/>
-      <c r="O551" s="4" t="n"/>
-      <c r="P551" s="4" t="n"/>
-      <c r="Q551" s="4" t="n"/>
-      <c r="R551" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S551" s="4" t="n"/>
-      <c r="T551" s="4" t="n"/>
-      <c r="U551" s="4" t="inlineStr">
+      <c r="E551" s="3" t="n"/>
+      <c r="F551" s="3" t="n"/>
+      <c r="G551" s="3" t="n"/>
+      <c r="H551" s="3" t="n"/>
+      <c r="I551" s="3" t="n"/>
+      <c r="J551" s="3" t="n"/>
+      <c r="K551" s="3" t="n"/>
+      <c r="L551" s="3" t="n"/>
+      <c r="M551" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N551" s="3" t="n"/>
+      <c r="O551" s="3" t="n"/>
+      <c r="P551" s="3" t="n"/>
+      <c r="Q551" s="3" t="n"/>
+      <c r="R551" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S551" s="3" t="n"/>
+      <c r="T551" s="3" t="n"/>
+      <c r="U551" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V551" s="4" t="inlineStr">
+      <c r="V551" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W551" s="4" t="n"/>
-      <c r="X551" s="4" t="n"/>
+      <c r="W551" s="3" t="n"/>
+      <c r="X551" s="3" t="n"/>
     </row>
     <row r="552">
       <c r="A552" s="2" t="inlineStr">
@@ -36881,62 +36881,62 @@
       <c r="X609" s="2" t="n"/>
     </row>
     <row r="610">
-      <c r="A610" s="4" t="inlineStr">
+      <c r="A610" s="3" t="inlineStr">
         <is>
           <t>BCIO:050267</t>
         </is>
       </c>
-      <c r="B610" s="4" t="inlineStr">
+      <c r="B610" s="3" t="inlineStr">
         <is>
           <t>uniform process aggregate</t>
         </is>
       </c>
-      <c r="C610" s="4" t="inlineStr">
+      <c r="C610" s="3" t="inlineStr">
         <is>
           <t>A process aggregate whose member parts are of the same type.</t>
         </is>
       </c>
-      <c r="D610" s="4" t="inlineStr">
+      <c r="D610" s="3" t="inlineStr">
         <is>
           <t>process aggregate</t>
         </is>
       </c>
-      <c r="E610" s="4" t="n"/>
-      <c r="F610" s="4" t="n"/>
-      <c r="G610" s="4" t="n"/>
-      <c r="H610" s="4" t="n"/>
-      <c r="I610" s="4" t="n"/>
-      <c r="J610" s="4" t="n"/>
-      <c r="K610" s="4" t="n"/>
-      <c r="L610" s="4" t="n"/>
-      <c r="M610" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N610" s="4" t="n"/>
-      <c r="O610" s="4" t="n"/>
-      <c r="P610" s="4" t="n"/>
-      <c r="Q610" s="4" t="n"/>
-      <c r="R610" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S610" s="4" t="n"/>
-      <c r="T610" s="4" t="n"/>
-      <c r="U610" s="4" t="inlineStr">
+      <c r="E610" s="3" t="n"/>
+      <c r="F610" s="3" t="n"/>
+      <c r="G610" s="3" t="n"/>
+      <c r="H610" s="3" t="n"/>
+      <c r="I610" s="3" t="n"/>
+      <c r="J610" s="3" t="n"/>
+      <c r="K610" s="3" t="n"/>
+      <c r="L610" s="3" t="n"/>
+      <c r="M610" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N610" s="3" t="n"/>
+      <c r="O610" s="3" t="n"/>
+      <c r="P610" s="3" t="n"/>
+      <c r="Q610" s="3" t="n"/>
+      <c r="R610" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S610" s="3" t="n"/>
+      <c r="T610" s="3" t="n"/>
+      <c r="U610" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V610" s="4" t="inlineStr">
+      <c r="V610" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W610" s="4" t="n"/>
-      <c r="X610" s="4" t="n"/>
+      <c r="W610" s="3" t="n"/>
+      <c r="X610" s="3" t="n"/>
     </row>
     <row r="611">
       <c r="A611" s="2" t="inlineStr">
@@ -37292,62 +37292,62 @@
       <c r="X616" s="2" t="n"/>
     </row>
     <row r="617">
-      <c r="A617" s="4" t="inlineStr">
+      <c r="A617" s="3" t="inlineStr">
         <is>
           <t>BCIO:050797</t>
         </is>
       </c>
-      <c r="B617" s="4" t="inlineStr">
+      <c r="B617" s="3" t="inlineStr">
         <is>
           <t>wider community behavioural consequence</t>
         </is>
       </c>
-      <c r="C617" s="4" t="inlineStr">
+      <c r="C617" s="3" t="inlineStr">
         <is>
           <t>A &lt;social behavioural consequence&gt; that is beyond the person’s family.</t>
         </is>
       </c>
-      <c r="D617" s="4" t="inlineStr">
+      <c r="D617" s="3" t="inlineStr">
         <is>
           <t>social behavioural consequence</t>
         </is>
       </c>
-      <c r="E617" s="4" t="n"/>
-      <c r="F617" s="4" t="n"/>
-      <c r="G617" s="4" t="n"/>
-      <c r="H617" s="4" t="n"/>
-      <c r="I617" s="4" t="n"/>
-      <c r="J617" s="4" t="n"/>
-      <c r="K617" s="4" t="n"/>
-      <c r="L617" s="4" t="n"/>
-      <c r="M617" s="4" t="inlineStr">
-        <is>
-          <t>Mechanisms of action</t>
-        </is>
-      </c>
-      <c r="N617" s="4" t="n"/>
-      <c r="O617" s="4" t="n"/>
-      <c r="P617" s="4" t="n"/>
-      <c r="Q617" s="4" t="n"/>
-      <c r="R617" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S617" s="4" t="n"/>
-      <c r="T617" s="4" t="n"/>
-      <c r="U617" s="4" t="inlineStr">
+      <c r="E617" s="3" t="n"/>
+      <c r="F617" s="3" t="n"/>
+      <c r="G617" s="3" t="n"/>
+      <c r="H617" s="3" t="n"/>
+      <c r="I617" s="3" t="n"/>
+      <c r="J617" s="3" t="n"/>
+      <c r="K617" s="3" t="n"/>
+      <c r="L617" s="3" t="n"/>
+      <c r="M617" s="3" t="inlineStr">
+        <is>
+          <t>Mechanisms of action</t>
+        </is>
+      </c>
+      <c r="N617" s="3" t="n"/>
+      <c r="O617" s="3" t="n"/>
+      <c r="P617" s="3" t="n"/>
+      <c r="Q617" s="3" t="n"/>
+      <c r="R617" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S617" s="3" t="n"/>
+      <c r="T617" s="3" t="n"/>
+      <c r="U617" s="3" t="inlineStr">
         <is>
           <t>PS</t>
         </is>
       </c>
-      <c r="V617" s="4" t="inlineStr">
+      <c r="V617" s="3" t="inlineStr">
         <is>
           <t>Obsolete</t>
         </is>
       </c>
-      <c r="W617" s="4" t="n"/>
-      <c r="X617" s="4" t="n"/>
+      <c r="W617" s="3" t="n"/>
+      <c r="X617" s="3" t="n"/>
     </row>
     <row r="618">
       <c r="A618" s="2" t="inlineStr">

</xml_diff>